<commit_message>
Update roomPerDay, roomArrangement, teacherArrangement
</commit_message>
<xml_diff>
--- a/Database/New Data _ 20150608/ClassCourse.xlsx
+++ b/Database/New Data _ 20150608/ClassCourse.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="89">
   <si>
     <t>Lớp</t>
   </si>
@@ -231,6 +231,57 @@
   </si>
   <si>
     <t>IBA1001</t>
+  </si>
+  <si>
+    <t>FIN0803</t>
+  </si>
+  <si>
+    <t>COF0803</t>
+  </si>
+  <si>
+    <t>COB0803</t>
+  </si>
+  <si>
+    <t>IBA0902</t>
+  </si>
+  <si>
+    <t>MKT0902</t>
+  </si>
+  <si>
+    <t>FIN303</t>
+  </si>
+  <si>
+    <t>FIN301</t>
+  </si>
+  <si>
+    <t>MAS201</t>
+  </si>
+  <si>
+    <t>ENM301</t>
+  </si>
+  <si>
+    <t>CHN122</t>
+  </si>
+  <si>
+    <t>BKG201</t>
+  </si>
+  <si>
+    <t>SSC101</t>
+  </si>
+  <si>
+    <t>MKT202</t>
+  </si>
+  <si>
+    <t>MKT301</t>
+  </si>
+  <si>
+    <t>CHN132</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MKT202 </t>
+  </si>
+  <si>
+    <t>ENM401</t>
   </si>
 </sst>
 </file>
@@ -319,7 +370,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
@@ -328,8 +379,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
@@ -361,8 +413,17 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 11" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
@@ -371,6 +432,7 @@
     <cellStyle name="Normal 4_QD578_13112012_BFU Bachelor Program for Spring  2013 V4-Final" xfId="5"/>
     <cellStyle name="Normal 7" xfId="6"/>
     <cellStyle name="Normal 8" xfId="7"/>
+    <cellStyle name="Normal_Full BSE programs_11-2010" xfId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -672,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1220,6 +1282,106 @@
         <v>69</v>
       </c>
     </row>
+    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>